<commit_message>
Completes PBCoreDigitalInstantiation upload Mapper
</commit_message>
<xml_diff>
--- a/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/digital_instantiation_manifest.xlsx
+++ b/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/digital_instantiation_manifest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason_corum/Code/ams/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD1F3916-A20C-0043-9528-15C417259064}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{903A7B55-1FD6-F840-84AF-8C5E51FFA0FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14520" xr2:uid="{6E11F67D-8A49-2B44-8162-C4263CE4169A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{6E11F67D-8A49-2B44-8162-C4263CE4169A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>DigitalInstantiation.filename</t>
   </si>
@@ -38,9 +33,6 @@
     <t>Asset.id</t>
   </si>
   <si>
-    <t>DigitalInstantiation.holding_institution</t>
-  </si>
-  <si>
     <t>DigitalInstantiation.generations</t>
   </si>
   <si>
@@ -63,6 +55,12 @@
   </si>
   <si>
     <t>disky mc diskface</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>DigitalInstantiation.location</t>
   </si>
 </sst>
 </file>
@@ -414,13 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFACFF4-0561-3E44-A5B1-CFCA2A32343D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,36 +428,42 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>123456</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP gets DigitalInstantiations to work
</commit_message>
<xml_diff>
--- a/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/digital_instantiation_manifest.xlsx
+++ b/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/digital_instantiation_manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason_corum/Code/ams/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{903A7B55-1FD6-F840-84AF-8C5E51FFA0FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881F8D62-3B74-BD42-9F2B-76B3EA589F0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{6E11F67D-8A49-2B44-8162-C4263CE4169A}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>Master</t>
   </si>
   <si>
-    <t>DigitalInstantiation.location</t>
+    <t>DigitalInstantiation.holding_organization</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adds test for md5
</commit_message>
<xml_diff>
--- a/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/digital_instantiation_manifest.xlsx
+++ b/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/digital_instantiation_manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason_corum/Code/ams/spec/fixtures/batch_ingest/sample_pbcore_digital_instantiation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881F8D62-3B74-BD42-9F2B-76B3EA589F0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB5160E-26BD-F942-AFDB-9750C1AC0D41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{6E11F67D-8A49-2B44-8162-C4263CE4169A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>DigitalInstantiation.filename</t>
   </si>
@@ -36,12 +36,6 @@
     <t>DigitalInstantiation.generations</t>
   </si>
   <si>
-    <t>DigitalInstantition.aapb_preservation_disk</t>
-  </si>
-  <si>
-    <t>DigitalInstantition.aapb_preservation_lto</t>
-  </si>
-  <si>
     <t>sample_digital_instantiation.xml</t>
   </si>
   <si>
@@ -61,6 +55,18 @@
   </si>
   <si>
     <t>DigitalInstantiation.holding_organization</t>
+  </si>
+  <si>
+    <t>qwertyqwerty</t>
+  </si>
+  <si>
+    <t>DigitalInstantiation.md5</t>
+  </si>
+  <si>
+    <t>DigitalInstantiation.aapb_preservation_lto</t>
+  </si>
+  <si>
+    <t>DigitalInstantiation.aapb_preservation_disk</t>
   </si>
 </sst>
 </file>
@@ -412,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFACFF4-0561-3E44-A5B1-CFCA2A32343D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,36 +440,42 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2">
         <v>123456</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>